<commit_message>
Added and updated translations
</commit_message>
<xml_diff>
--- a/templates/language-kurz.xlsx
+++ b/templates/language-kurz.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Documents/Webpages/Unlabeler-Webpage-Deploy/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9036DFD-583C-AF4B-9D60-64130EA11681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13D12AF-A7D0-7D48-BB3F-4AF3FC2D13C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="1560" windowWidth="27840" windowHeight="16740" xr2:uid="{7E36295F-81ED-144A-B7D7-008660E6F8FE}"/>
+    <workbookView xWindow="18600" yWindow="4140" windowWidth="27840" windowHeight="16740" xr2:uid="{7E36295F-81ED-144A-B7D7-008660E6F8FE}"/>
   </bookViews>
   <sheets>
     <sheet name="language" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="en" localSheetId="0">language!$A$4:$C$127</definedName>
+    <definedName name="en" localSheetId="0">language!$A$4:$C$130</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="601">
   <si>
     <t>settings-text2</t>
   </si>
@@ -224,9 +224,6 @@
     <t xml:space="preserve">Quick-tap 6 points on the label (corners and top and bottom edges) </t>
   </si>
   <si>
-    <t xml:space="preserve">Press 'unlabel' to generate a perfectly rectangular label </t>
-  </si>
-  <si>
     <t xml:space="preserve">No more distorted labels in your tasting notes or collection! Just grab your perfect label shot and save it or share it wherever you want. </t>
   </si>
   <si>
@@ -296,9 +293,6 @@
     <t>If you want you can add a star rating to the label by clicking on the star button, tapping on the empty stars for a rating, choose your color scheme and add it.</t>
   </si>
   <si>
-    <t>Now you can save the unlabelled image to your phone by pressing the down arrow button, which stores it directly in your gallery.</t>
-  </si>
-  <si>
     <t>You can also share the perfectly rectangular label with other apps using the share icon, making it easy to add to your tasting notes or digital collection.</t>
   </si>
   <si>
@@ -416,9 +410,6 @@
     <t>How can I remove the watermark from the labels?</t>
   </si>
   <si>
-    <t>To remove the watermark, please buy the 'Pure Labels' in-app purchase. You can find the purchase option on the start or help page.</t>
-  </si>
-  <si>
     <t>Is there a dark mode for the app?</t>
   </si>
   <si>
@@ -428,9 +419,6 @@
     <t>&lt;span&gt;&amp;larr;&lt;/span&gt; App Settings</t>
   </si>
   <si>
-    <t>Once all marks are set, press the \unlabel\ button.</t>
-  </si>
-  <si>
     <t>'The Unlabeler':  Your solution for perfect bottle label photos!</t>
   </si>
   <si>
@@ -806,9 +794,6 @@
     <t>Wenn du möchtest, kannst du dem Etikett eine Sternebwertung hinzufügen, indem du auf die Stern-Schaltfläche klickst, passend auf die leeren Sterne für eine Bewertung tippst, dein Farbschema auswählst und die Bewertung hinzufügst.</t>
   </si>
   <si>
-    <t>Jetzt kannst du das 'abgelöste' Etikett auf deinem Handy speichern, indem du die Schaltfläche mit dem Pfeil nach unten drückst.</t>
-  </si>
-  <si>
     <t>Du kannst das perfekt rechteckige Etikett auch mit anderen Apps über das Teilen-Symbol teilen, um es z.B. zu deiner Tasting-App hinzuzufügen.</t>
   </si>
   <si>
@@ -953,9 +938,6 @@
     <t>Wie kann ich das Wasserzeichen von den Etiketten entfernen?</t>
   </si>
   <si>
-    <t>Um das Wasserzeichen zu entfernen, erwerbe bitte den 'Pure Labels'-In-App-Kauf. Du findest die Kaufoption auf der Start- oder Hilfeseite.</t>
-  </si>
-  <si>
     <t>Gibt es einen Dark Mode für die App?</t>
   </si>
   <si>
@@ -1028,9 +1010,6 @@
     <t>copyright</t>
   </si>
   <si>
-    <t>2025 by Mug of Coffee Software GmbH</t>
-  </si>
-  <si>
     <t>index_pagetitle</t>
   </si>
   <si>
@@ -1155,13 +1134,733 @@
   </si>
   <si>
     <t>it</t>
+  </si>
+  <si>
+    <t>Descargar</t>
+  </si>
+  <si>
+    <t>Scarica</t>
+  </si>
+  <si>
+    <t>Contacto</t>
+  </si>
+  <si>
+    <t>Contatto</t>
+  </si>
+  <si>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>Menú</t>
+  </si>
+  <si>
+    <t>Despega tus etiquetas digitalmente - perfectas, planas, rectangulares - sin distorsión, sin fondo molesto - para iPhone, iPad o Mac. Para amantes del vino o cerveza artesanal, sommeliers, entusiastas del gin o simplemente fans de 'Drops of God'</t>
+  </si>
+  <si>
+    <t>Stacca le tue etichette digitalmente - perfette, piatte, rettangolari - senza distorsione, senza sfondo fastidioso - per iPhone, iPad o Mac. Per amanti del vino o birra artigianale, sommelier, appassionati di gin o semplicemente fan di 'Drops of God'</t>
+  </si>
+  <si>
+    <t>Extrae una etiqueta sin distorsión de la foto de una botella con solo unos clics - ¡y guárdala o envíala a tu app favorita de cata o notas! Funciona en tu iPhone, iPad o Mac.</t>
+  </si>
+  <si>
+    <t>Estrai un'etichetta senza distorsione dalla foto di una bottiglia con solo pochi clic - e salvala o inviala alla tua app preferita per degustazioni o note! Funziona su iPhone, iPad o Mac.</t>
+  </si>
+  <si>
+    <t>¡La app imprescindible para entusiastas del vino, cerveza, whisky, gin, ... o incluso mermelada!</t>
+  </si>
+  <si>
+    <t>L'app indispensabile per appassionati di vino, birra, whisky, gin, ... o persino marmellata!</t>
+  </si>
+  <si>
+    <t>Resumen</t>
+  </si>
+  <si>
+    <t>Panoramica</t>
+  </si>
+  <si>
+    <t>Cómo Usarla</t>
+  </si>
+  <si>
+    <t>Come Usarla</t>
+  </si>
+  <si>
+    <t>Compras en la App</t>
+  </si>
+  <si>
+    <t>Acquisti In-App</t>
+  </si>
+  <si>
+    <t>Configuración</t>
+  </si>
+  <si>
+    <t>Impostazioni</t>
+  </si>
+  <si>
+    <t>Aviso Legal</t>
+  </si>
+  <si>
+    <t>Note Legali</t>
+  </si>
+  <si>
+    <t>Política de Privacidad</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Resumen</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Panoramica</t>
+  </si>
+  <si>
+    <t>El flujo de trabajo es súper simple y rápido - ¡toma una foto, solo unos clics, listo!</t>
+  </si>
+  <si>
+    <t>Il flusso di lavoro è super semplice e veloce - scatta una foto, solo pochi clic, fatto!</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>¿Eres un amante del vino o la cerveza y quieres guardar la etiqueta de esta maravillosa bebida que acabas de disfrutar para tus notas de cata? ¿Alguna vez has intentado fotografiar una bonita etiqueta, solo para obtener una imagen distorsionada que no representa correctamente el original, con una botella cortada y un fondo molesto? ¿O has intentado alguna vez mojar una botella, despegar la etiqueta, secarla y luego hacerle una foto?</t>
+  </si>
+  <si>
+    <t>Sei un amante del vino o della birra e vuoi conservare l'etichetta di questa meravigliosa bevanda che hai appena gustato per le tue note di degustazione? Hai mai provato a fotografare una bella etichetta, solo per ritrovarti con un'immagine distorta che non rappresenta correttamente l'originale, con una bottiglia tagliata e uno sfondo fastidioso? O hai mai provato a bagnare una bottiglia, staccare l'etichetta, asciugarla e poi fotografarla?</t>
+  </si>
+  <si>
+    <t>Descubre 'The Unlabeler' - para recuerdos digitales perfectos de tus bebidas.</t>
+  </si>
+  <si>
+    <t>Scopri 'The Unlabeler' - per ricordi digitali perfetti delle tue bevande.</t>
+  </si>
+  <si>
+    <t>Esta aplicación intuitiva transforma etiquetas de botellas distorsionadas por la perspectiva en imágenes bonitas y planas - perfectas para notas de cata, colecciones digitales o para compartir con tus amigos. Ya seas un entusiasta del vino, explorador de cerveza artesanal o conocedor de licores, es súper fácil de usar:</t>
+  </si>
+  <si>
+    <t>Questa applicazione intuitiva trasforma le etichette delle bottiglie distorte dalla prospettiva in immagini belle e piatte - perfette per note di degustazione, collezioni digitali o da condividere con i tuoi amici. Che tu sia un appassionato di vino, esploratore di birra artigianale o intenditore di liquori, è super semplice da usare:</t>
+  </si>
+  <si>
+    <t>Selecciona una foto de tu botella</t>
+  </si>
+  <si>
+    <t>Seleziona una foto della tua bottiglia</t>
+  </si>
+  <si>
+    <t>Toca rápidamente 6 puntos en la etiqueta (esquinas y bordes superior e inferior)</t>
+  </si>
+  <si>
+    <t>Tocca rapidamente 6 punti sull'etichetta (angoli e bordi superiore e inferiore)</t>
+  </si>
+  <si>
+    <t>¡No más etiquetas distorsionadas en tus notas de cata o colección! Simplemente toma tu etiqueta perfecta y guárdala o compártela donde quieras.</t>
+  </si>
+  <si>
+    <t>Basta etichette distorte nelle tue note di degustazione o collezione! Prendi semplicemente la tua etichetta perfetta e salvala o condividila dove vuoi.</t>
+  </si>
+  <si>
+    <t>'The Unlabeler': ¡Tu solución para fotos perfectas de etiquetas de botellas!</t>
+  </si>
+  <si>
+    <t>'The Unlabeler': La tua soluzione per foto perfette delle etichette delle bottiglie!</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;→&lt;/span&gt; Cómo Usar la App</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;→&lt;/span&gt; Come Usare l'App</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Cómo Usar la App</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Come Usare l'App</t>
+  </si>
+  <si>
+    <t>Ottieni una comprensione più profonda del flusso di lavoro, come zoomare, posizionare ed eliminare segni, staccare etichette, aggiungere una valutazione a stelle e condividere o salvare l'etichetta</t>
+  </si>
+  <si>
+    <t>Cómo Usar la App</t>
+  </si>
+  <si>
+    <t>Come Usare l'App</t>
+  </si>
+  <si>
+    <t>Comenzar con 'The Unlabeler' es tan simple como tomar una foto. Sigue estos sencillos pasos para transformar tus etiquetas distorsionadas por la perspectiva en recuerdos digitales perfectos:</t>
+  </si>
+  <si>
+    <t>Iniziare con 'The Unlabeler' è semplice come scattare una foto. Segui questi semplici passaggi per trasformare le tue etichette distorte dalla prospettiva in ricordi digitali perfetti:</t>
+  </si>
+  <si>
+    <t>Selecciona o Toma una Foto</t>
+  </si>
+  <si>
+    <t>Seleziona o Scatta una Foto</t>
+  </si>
+  <si>
+    <t>En la primera pantalla, toma una foto de tu botella o elige una de tu galería.</t>
+  </si>
+  <si>
+    <t>Nella prima schermata, scatta una foto della tua bottiglia o scegline una dalla tua galleria.</t>
+  </si>
+  <si>
+    <t>Asegúrate de que la etiqueta sea claramente visible y lo más grande posible contra un fondo contrastante.</t>
+  </si>
+  <si>
+    <t>Assicurati che l'etichetta sia chiaramente visibile e il più grande possibile contro uno sfondo contrastante.</t>
+  </si>
+  <si>
+    <t>Si es posible, usa un zoom teleobjetivo y no un lente gran angular para evitar distorsión adicional.</t>
+  </si>
+  <si>
+    <t>Se possibile, usa uno zoom teleobiettivo e non un obiettivo grandangolare per evitare distorsioni aggiuntive.</t>
+  </si>
+  <si>
+    <t>Esto ayuda a la app a procesar y transformar la etiqueta con precisión.</t>
+  </si>
+  <si>
+    <t>Questo aiuta l'app a elaborare e trasformare accuratamente l'etichetta.</t>
+  </si>
+  <si>
+    <t>Marca la Etiqueta</t>
+  </si>
+  <si>
+    <t>Segna l'Etichetta</t>
+  </si>
+  <si>
+    <t>En la siguiente pantalla, toca rápidamente para marcar las cuatro esquinas y (aproximadamente) el centro de los bordes superior e inferior de la etiqueta.</t>
+  </si>
+  <si>
+    <t>Nella schermata successiva, tocca rapidamente per segnare i quattro angoli e (approssimativamente) il centro dei bordi superiore e inferiore dell'etichetta.</t>
+  </si>
+  <si>
+    <t>Puedes arrastrar la imagen con un dedo y hacer zoom con dos dedos o los botones de zoom para ver los detalles.</t>
+  </si>
+  <si>
+    <t>Puoi trascinare l'immagine con un dito e fare zoom avanti o indietro con due dita o i pulsanti di zoom per vedere i dettagli.</t>
+  </si>
+  <si>
+    <t>Para mayor precisión, usa la lupa en la parte inferior para obtener una vista más cercana de cada punto.</t>
+  </si>
+  <si>
+    <t>Per maggiore precisione, usa la lente d'ingrandimento in basso per ottenere una vista più ravvicinata di ogni punto.</t>
+  </si>
+  <si>
+    <t>Posiciona la esquina superior izquierda de la etiqueta en el área ampliada y toca para marcarla.</t>
+  </si>
+  <si>
+    <t>Posiziona l'angolo superiore sinistro dell'etichetta nell'area ingrandita e tocca per contrassegnarlo.</t>
+  </si>
+  <si>
+    <t>Luego, marca el centro del borde superior y la esquina superior derecha. Repite este proceso para el borde inferior.</t>
+  </si>
+  <si>
+    <t>Quindi, segna il centro del bordo superiore e l'angolo superiore destro. Ripeti questo processo per il bordo inferiore.</t>
+  </si>
+  <si>
+    <t>La secuencia no importa -- solo asegúrate de que los seis puntos estén marcados con precisión.</t>
+  </si>
+  <si>
+    <t>La sequenza non importa -- assicurati solo che tutti e sei i punti siano contrassegnati accuratamente.</t>
+  </si>
+  <si>
+    <t>Ajusta las Marcas</t>
+  </si>
+  <si>
+    <t>Regola i Segni</t>
+  </si>
+  <si>
+    <t>Si necesitas corregir una marca, simplemente toca el botón de borrador para eliminar la última marca que colocaste.</t>
+  </si>
+  <si>
+    <t>Se devi correggere un segno, tocca semplicemente il pulsante gomma per eliminare l'ultimo segno che hai posizionato.</t>
+  </si>
+  <si>
+    <t>Alternativamente, puedes tocar una marca específica para seleccionarla y luego presionar el botón de borrador para eliminarla.</t>
+  </si>
+  <si>
+    <t>In alternativa, puoi toccare un segno specifico per selezionarlo e poi premere il pulsante gomma per rimuoverlo.</t>
+  </si>
+  <si>
+    <t>Esta característica asegura que puedas hacer ajustes fácilmente sin empezar de nuevo.</t>
+  </si>
+  <si>
+    <t>Questa funzione garantisce che tu possa fare regolazioni facilmente senza ricominciare da capo.</t>
+  </si>
+  <si>
+    <t>Quita la Etiqueta</t>
+  </si>
+  <si>
+    <t>Stacca l'Etichetta</t>
+  </si>
+  <si>
+    <t>La app realizará un cálculo rápido para corregir la distorsión de perspectiva.</t>
+  </si>
+  <si>
+    <t>L'app eseguirà un calcolo rapido per correggere la distorsione prospettica.</t>
+  </si>
+  <si>
+    <t>En unos momentos, verás la etiqueta transformada mostrada en la siguiente pantalla.</t>
+  </si>
+  <si>
+    <t>In pochi istanti, vedrai l'etichetta trasformata visualizzata nella schermata successiva.</t>
+  </si>
+  <si>
+    <t>Añade una Calificación de Estrellas, Guarda o Comparte</t>
+  </si>
+  <si>
+    <t>Aggiungi una Valutazione a Stelle, Salva o Condividi</t>
+  </si>
+  <si>
+    <t>Si quieres, puedes añadir una calificación de estrellas a la etiqueta haciendo clic en el botón de estrella, tocando las estrellas vacías para una calificación, eligiendo tu esquema de color y añadiéndola.</t>
+  </si>
+  <si>
+    <t>Se vuoi, puoi aggiungere una valutazione a stelle all'etichetta cliccando sul pulsante stella, toccando le stelle vuote per una valutazione, scegliendo la tua combinazione di colori e aggiungendola.</t>
+  </si>
+  <si>
+    <t>También puedes compartir la etiqueta perfectamente rectangular con otras apps usando el ícono de compartir, facilitando añadirla a tus notas de cata o colección digital.</t>
+  </si>
+  <si>
+    <t>Puoi anche condividere l'etichetta perfettamente rettangolare con altre app usando l'icona di condivisione, rendendo facile aggiungerla alle tue note di degustazione o collezione digitale.</t>
+  </si>
+  <si>
+    <t>Si quieres quitar otra etiqueta, toca el ícono más para comenzar el proceso nuevamente.</t>
+  </si>
+  <si>
+    <t>Se vuoi staccare un'altra etichetta, tocca l'icona più per iniziare nuovamente il processo.</t>
+  </si>
+  <si>
+    <t>Si alguna marca necesita más ajustes, simplemente toca el botón de atrás (chevron en la esquina superior izquierda) para refinarlas.</t>
+  </si>
+  <si>
+    <t>Se alcuni segni necessitano di ulteriori regolazioni, tocca semplicemente il pulsante indietro (chevron nell'angolo superiore sinistro) per perfezionarli.</t>
+  </si>
+  <si>
+    <t>Con 'The Unlabeler', capturar fotos perfectas de etiquetas nunca ha sido más fácil. Transforma las etiquetas de tus botellas en imágenes digitales impecables y compártelas con facilidad. Ya sea que las añadas a tus notas de cata, colecciones digitales o simplemente las compartas con amigos, 'The Unlabeler' asegura que los recuerdos de tus bebidas favoritas se vean en su mejor forma.</t>
+  </si>
+  <si>
+    <t>Con 'The Unlabeler', catturare foto perfette delle etichette non è mai stato così facile. Trasforma le etichette delle tue bottiglie in immagini digitali impeccabili e condividile con facilità. Che tu le stia aggiungendo alle tue note di degustazione, collezioni digitali o semplicemente condividendole con gli amici, 'The Unlabeler' garantisce che i ricordi delle tue bevande preferite appaiano al meglio.</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;←&lt;/span&gt; Resumen</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;←&lt;/span&gt; Panoramica</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;→&lt;/span&gt; Compras en la App</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;→&lt;/span&gt; Acquisti In-App</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Configuración de la App</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Impostazioni App</t>
+  </si>
+  <si>
+    <t>Optimiza 'The Unlabeler' con estas configuraciones</t>
+  </si>
+  <si>
+    <t>Ottimizza 'The Unlabeler' con queste impostazioni</t>
+  </si>
+  <si>
+    <t>Configuración de la App</t>
+  </si>
+  <si>
+    <t>Impostazioni App</t>
+  </si>
+  <si>
+    <t>Acceder a la configuración de 'The Unlabeler' es sencillo. Toca el ícono de engranaje ubicado en la esquina superior derecha de la pantalla para personalizar tu experiencia:</t>
+  </si>
+  <si>
+    <t>Accedere alle impostazioni di 'The Unlabeler' è semplice. Tocca l'icona dell'ingranaggio situata nell'angolo superiore destro dello schermo per personalizzare la tua esperienza:</t>
+  </si>
+  <si>
+    <t>Operación para Zurdos</t>
+  </si>
+  <si>
+    <t>Operazione per Mancini</t>
+  </si>
+  <si>
+    <t>: Para usuarios zurdos, puedes duplicar los botones en la parte inferior del lado derecho al lado izquierdo habilitando 'operación para zurdos'. Esto hace que la app sea más cómoda e intuitiva de usar.</t>
+  </si>
+  <si>
+    <t>: Per gli utenti mancini, puoi specchiare i pulsanti in basso dal lato destro al lato sinistro attivando 'operazione per mancini'. Questo rende l'app più comoda e intuitiva da usare.</t>
+  </si>
+  <si>
+    <t>Mostrar Botones de Zoom</t>
+  </si>
+  <si>
+    <t>Mostra Pulsanti Zoom</t>
+  </si>
+  <si>
+    <t>: Muestra botones de zoom adicionales en el lado derecho de la pantalla. Puedes hacer zoom con dos dedos en cualquier caso.</t>
+  </si>
+  <si>
+    <t>: Mostra pulsanti di zoom aggiuntivi sul lato destro dello schermo. Puoi fare zoom con due dita in ogni caso.</t>
+  </si>
+  <si>
+    <t>Guardar Foto de Cámara</t>
+  </si>
+  <si>
+    <t>Salva Foto Fotocamera</t>
+  </si>
+  <si>
+    <t>: Si tomas una foto directamente con la cámara, puedes elegir si la foto debe guardarse en la biblioteca de fotos o no. Si no la guardas, solo se usará para quitar etiquetas.</t>
+  </si>
+  <si>
+    <t>: Se scatti una foto direttamente con la fotocamera, puoi scegliere se la foto deve essere salvata nella libreria foto o no. Se non la salvi, verrà usata solo per staccare etichette.</t>
+  </si>
+  <si>
+    <t>Las siguientes configuraciones solo están disponibles si has comprado el 'Paquete Sommelier'.</t>
+  </si>
+  <si>
+    <t>Le seguenti impostazioni sono disponibili solo se hai acquistato il 'Pacchetto Sommelier'.</t>
+  </si>
+  <si>
+    <t>Opciones de Ancho de Etiqueta</t>
+  </si>
+  <si>
+    <t>Opzioni Larghezza Etichetta</t>
+  </si>
+  <si>
+    <t>: Personaliza cómo la app maneja el ancho de tus imágenes sin etiqueta. Hay tres configuraciones diferentes</t>
+  </si>
+  <si>
+    <t>: Personalizza come l'app gestisce la larghezza delle tue immagini senza etichetta. Ci sono tre impostazioni diverse</t>
+  </si>
+  <si>
+    <t>Ilimitado</t>
+  </si>
+  <si>
+    <t>Illimitato</t>
+  </si>
+  <si>
+    <t>: El ancho de la etiqueta se ajusta automáticamente para ser proporcional a su altura en la foto, sin restricciones.</t>
+  </si>
+  <si>
+    <t>: La larghezza dell'etichetta viene regolata automaticamente per essere proporzionale alla sua altezza nella foto, senza restrizioni.</t>
+  </si>
+  <si>
+    <t>Limitado</t>
+  </si>
+  <si>
+    <t>Limitato</t>
+  </si>
+  <si>
+    <t>: El ancho se ajusta proporcionalmente a la altura, pero si supera un límite establecido, la etiqueta se reducirá para que quepa dentro de ese límite.</t>
+  </si>
+  <si>
+    <t>: La larghezza viene regolata proporzionalmente all'altezza, ma se supera un limite prestabilito, l'etichetta verrà ridimensionata per rientrare in quel limite.</t>
+  </si>
+  <si>
+    <t>Fijo</t>
+  </si>
+  <si>
+    <t>Fisso</t>
+  </si>
+  <si>
+    <t>: La etiqueta se escala para que coincida exactamente con un ancho específico. Esta opción es especialmente útil para mantener una presentación consistente en tu app de cata, ya que todas las etiquetas tendrán el mismo ancho, proporcionando un aspecto claro y uniforme.</t>
+  </si>
+  <si>
+    <t>: L'etichetta viene ridimensionata per corrispondere esattamente a una larghezza specifica. Questa opzione è particolarmente utile per mantenere una presentazione coerente nella tua app di degustazione, poiché tutte le etichette avranno la stessa larghezza, fornendo un aspetto chiaro e uniforme.</t>
+  </si>
+  <si>
+    <t>Puedes establecer el límite para las opciones 'Limitado' y 'Fijo' en el campo de entrada, eligiendo un valor entre 300 y 5000 píxeles que se adapte a tus necesidades.</t>
+  </si>
+  <si>
+    <t>Puoi impostare il limite per le opzioni 'Limitato' e 'Fisso' nel campo di input, scegliendo un valore tra 300 e 5000 pixel che si adatti alle tue esigenze.</t>
+  </si>
+  <si>
+    <t>Nombre del archivo de la etiqueta compartida</t>
+  </si>
+  <si>
+    <t>Nome del file dell'etichetta condivisa</t>
+  </si>
+  <si>
+    <t>: Puedes especificar el nombre del archivo de la etiqueta compartida. El nombre predeterminado es 'TuEtiqueta.jpg'.</t>
+  </si>
+  <si>
+    <t>: Puoi specificare il nome del file dell'etichetta condivisa. Il nome predefinito è 'TuaEtichetta.jpg'.</t>
+  </si>
+  <si>
+    <t>Álbum Unlabeler</t>
+  </si>
+  <si>
+    <t>Album Unlabeler</t>
+  </si>
+  <si>
+    <t>: Puedes guardar la etiqueta en el álbum 'TheUnlabeler'. Si el álbum no existe, se creará automáticamente.</t>
+  </si>
+  <si>
+    <t>: Puoi salvare l'etichetta nell'album 'TheUnlabeler'. Se l'album non esiste, verrà creato automaticamente.</t>
+  </si>
+  <si>
+    <t>Animación de despegado</t>
+  </si>
+  <si>
+    <t>Animazione di rimozione</t>
+  </si>
+  <si>
+    <t>: Después de presionar el botón 'despegar' verás una animación hasta que se calcule tu etiqueta final. Dependiendo de la velocidad de tu dispositivo y el tamaño de la etiqueta, el cálculo normalmente es más rápido que la animación, por lo que solo verás el principio. Si quieres ver la animación completa puedes activar esta configuración.</t>
+  </si>
+  <si>
+    <t>: Dopo aver premuto il pulsante 'rimuovi' vedrai un'animazione fino a quando la tua etichetta finale sarà calcolata. A seconda della velocità del tuo dispositivo e delle dimensioni dell'etichetta, il calcolo è normalmente più veloce dell'animazione, quindi vedrai solo l'inizio. Se vuoi vedere l'animazione completa puoi attivare questa impostazione.</t>
+  </si>
+  <si>
+    <t>Estas configuraciones te permiten adaptar 'The Unlabeler' a tus preferencias, asegurando que captures la foto perfecta de la etiqueta cada vez.</t>
+  </si>
+  <si>
+    <t>Queste impostazioni ti permettono di personalizzare 'The Unlabeler' secondo le tue preferenze, assicurandoti di catturare ogni volta la foto perfetta dell'etichetta.</t>
+  </si>
+  <si>
+    <t>Configuración básica</t>
+  </si>
+  <si>
+    <t>Impostazioni di base</t>
+  </si>
+  <si>
+    <t>Paquete Sommelier</t>
+  </si>
+  <si>
+    <t>Pacchetto Sommelier</t>
+  </si>
+  <si>
+    <t>../assets/img/Settings-es.png</t>
+  </si>
+  <si>
+    <t>../assets/img/Settings-it.png</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;←&lt;/span&gt; Compras en la app</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;←&lt;/span&gt; Acquisti in-app</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;→&lt;/span&gt; App Store</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Compras en la app</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Acquisti in-app</t>
+  </si>
+  <si>
+    <t>Compras en la app</t>
+  </si>
+  <si>
+    <t>Acquisti in-app</t>
+  </si>
+  <si>
+    <t>VERSIÓN GRATUITA</t>
+  </si>
+  <si>
+    <t>VERSIONE GRATUITA</t>
+  </si>
+  <si>
+    <t>Con la versión gratuita de 'The Unlabeler' puedes despegar y guardar tantas etiquetas como quieras, pero se añadirá una pequeña marca de agua a todas las etiquetas. ¡Solo pruébalo y quedarás convencido!</t>
+  </si>
+  <si>
+    <t>Con la versione gratuita di 'The Unlabeler' puoi rimuovere e salvare tutte le etichette che vuoi, ma verrà aggiunta una piccola filigrana a tutte le etichette. Provalo e rimarrai convinto!</t>
+  </si>
+  <si>
+    <t>PAQUETE SOMMELIER</t>
+  </si>
+  <si>
+    <t>PACCHETTO SOMMELIER</t>
+  </si>
+  <si>
+    <t>Para usuarios avanzados, está el 'PAQUETE SOMMELIER' que desbloquea una variedad de funciones avanzadas como:</t>
+  </si>
+  <si>
+    <t>Per gli utenti esperti, c'è il 'PACCHETTO SOMMELIER' che sblocca una varietà di funzioni avanzate come:</t>
+  </si>
+  <si>
+    <t>Guardar tus etiquetas en un álbum separado,</t>
+  </si>
+  <si>
+    <t>Salvare le tue etichette in un album separato,</t>
+  </si>
+  <si>
+    <t>Usar un nombre personalizable para etiquetas compartidas,</t>
+  </si>
+  <si>
+    <t>Usare un nome personalizzabile per le etichette condivise,</t>
+  </si>
+  <si>
+    <t>Establecer un tamaño de píxel fijo para todas las etiquetas, para que tengan el mismo ancho en tu app de cata,</t>
+  </si>
+  <si>
+    <t>Impostare una dimensione pixel fissa per tutte le etichette, così hanno la stessa larghezza nella tua app di degustazione,</t>
+  </si>
+  <si>
+    <t>Hacer zoom en la etiqueta final para verificar su calidad,</t>
+  </si>
+  <si>
+    <t>Fare zoom sull'etichetta finale per controllarne la qualità,</t>
+  </si>
+  <si>
+    <t>Añadir una calificación de estrellas a la etiqueta final, y más.</t>
+  </si>
+  <si>
+    <t>Aggiungere una valutazione a stelle all'etichetta finale, e altro ancora.</t>
+  </si>
+  <si>
+    <t>Todas las compras en la app son compras únicas. Sin suscripciones ni tarifas ocultas.</t>
+  </si>
+  <si>
+    <t>Tutti gli acquisti in-app sono acquisti una tantum. Nessun abbonamento o commissione nascosta.</t>
+  </si>
+  <si>
+    <t>La app funciona en iPhone, iPad y Mac con las mismas compras en la app.</t>
+  </si>
+  <si>
+    <t>L'app funziona su iPhone, iPad e Mac con gli stessi acquisti in-app.</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;←&lt;/span&gt; Cómo usar la app</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;←&lt;/span&gt; Come usare l'app</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;→&lt;/span&gt; Configuración de la app</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;→&lt;/span&gt; Impostazioni dell'app</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Preguntas frecuentes - FAQ</t>
+  </si>
+  <si>
+    <t>The Unlabeler - Domande frequenti - FAQ</t>
+  </si>
+  <si>
+    <t>Obtén la respuesta a tus preguntas</t>
+  </si>
+  <si>
+    <t>Ottieni la risposta alle tue domande</t>
+  </si>
+  <si>
+    <t>Aquí están tus preguntas frecuentes:</t>
+  </si>
+  <si>
+    <t>Ecco le tue domande frequenti:</t>
+  </si>
+  <si>
+    <t>¿Hay restricciones para la forma de la etiqueta y la botella?</t>
+  </si>
+  <si>
+    <t>Ci sono restrizioni per la forma dell'etichetta e della bottiglia?</t>
+  </si>
+  <si>
+    <t>Sí, la app Unlabeler puede corregir la distorsión de etiquetas rectangulares en botellas cilíndricas, lo cual aplica a la mayoría de botellas estándar.</t>
+  </si>
+  <si>
+    <t>Sì, l'app Unlabeler può correggere la distorsione di etichette rettangolari su bottiglie cilindriche, che si applica alla maggior parte delle bottiglie standard.</t>
+  </si>
+  <si>
+    <t>Si tu etiqueta tiene una forma diferente, simplemente usa las 6 marcas para marcar un área que encierre y que pueda corresponder a una etiqueta rectangular y despégala.</t>
+  </si>
+  <si>
+    <t>Se la tua etichetta ha una forma diversa, usa semplicemente i 6 segni per marcare un'area che racchiuda e che possa corrispondere a un'etichetta rettangolare e rimuovila.</t>
+  </si>
+  <si>
+    <t>¿Cómo puedo quitar la marca de agua de las etiquetas?</t>
+  </si>
+  <si>
+    <t>Come posso rimuovere la filigrana dalle etichette?</t>
+  </si>
+  <si>
+    <t>¿Hay un modo oscuro para la app?</t>
+  </si>
+  <si>
+    <t>C'è una modalità scura per l'app?</t>
+  </si>
+  <si>
+    <t>Sí, absolutamente. ¡Pruébalo y disfruta del nuevo aspecto!</t>
+  </si>
+  <si>
+    <t>Sì, assolutamente. Provalo e goditi il nuovo aspetto!</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;←&lt;/span&gt; Configuración de la app</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;←&lt;/span&gt; Impostazioni dell'app</t>
+  </si>
+  <si>
+    <t>2026 by Mug of Coffee Software GmbH</t>
+  </si>
+  <si>
+    <t>Once all marks are set, press the 'Unlabel' button.</t>
+  </si>
+  <si>
+    <t>Una vez que todas las marcas estén establecidas, presiona el botón 'Unlabel'.</t>
+  </si>
+  <si>
+    <t>Una volta che tutti i segni sono impostati, premi il pulsante 'Unlabel'.</t>
+  </si>
+  <si>
+    <t>Now you can save the unlabelled label to your phone by pressing the down arrow button, which stores it directly in your gallery.</t>
+  </si>
+  <si>
+    <t>Jetzt kannst du das 'abgelöste' Etikett auf deinem Handy in der Galerie speichern, indem du die Schaltfläche mit dem Pfeil nach unten drückst.</t>
+  </si>
+  <si>
+    <t>Ahora puedes guardar la etiqueta despegada en la galería de tu móvil pulsando el botón con la flecha hacia abajo.</t>
+  </si>
+  <si>
+    <t>Ora puoi salvare l'etichetta staccata nella galleria del tuo cellulare premendo il pulsante con la freccia rivolta verso il basso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Press 'Unlabel' to generate a perfectly rectangular label </t>
+  </si>
+  <si>
+    <t>Presiona 'Unlabel' para generar una etiqueta perfectamente rectangular</t>
+  </si>
+  <si>
+    <t>Premi 'Unlabel' per generare un'etichetta perfettamente rettangolare</t>
+  </si>
+  <si>
+    <t>Obtén una comprensión más profunda del flujo de trabajo, cómo hacer zoom, colocar y eliminar marcas, despegar la etiqueta, añadir una calificación de estrellas y compartir o guardar la etiqueta</t>
+  </si>
+  <si>
+    <t>Desbloquea todo el potencial de 'The Unlabeler' con ETIQUETAS PURAS y el PAQUETE SOMMELIER</t>
+  </si>
+  <si>
+    <t>Sblocca tutto il potenziale di 'The Unlabeler' con ETICHETTE PURE e il PACCHETTO SOMMELIER</t>
+  </si>
+  <si>
+    <t>ETIQUETAS PURAS</t>
+  </si>
+  <si>
+    <t>ETICHETTE PURE</t>
+  </si>
+  <si>
+    <t>Con la compra en la app 'ETIQUETAS PURAS' puedes disfrutar de todas tus futuras etiquetas sin una marca de agua molesta.</t>
+  </si>
+  <si>
+    <t>Con l'acquisto in-app 'ETICHETTE PURE' puoi goderti tutte le tue future etichette senza una filigrana fastidiosa.</t>
+  </si>
+  <si>
+    <t>To remove the watermark, please buy the 'PURE LABELS' in-app purchase. You can find the purchase option on the start or help page.</t>
+  </si>
+  <si>
+    <t>Um das Wasserzeichen zu entfernen, erwerbe bitte den 'PURE LABELS'-In-App-Kauf. Du findest die Kaufoption auf der Start- oder Hilfeseite.</t>
+  </si>
+  <si>
+    <t>Para quitar la marca de agua, por favor compra la compra en la app 'ETIQUETAS PURAS'. Puedes encontrar la opción de compra en la página de inicio o ayuda.</t>
+  </si>
+  <si>
+    <t>Per rimuovere la filigrana, acquista l'acquisto in-app 'ETICHETTE PURE'. Puoi trovare l'opzione di acquisto nella pagina iniziale o di aiuto.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1171,6 +1870,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1196,12 +1903,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1524,1113 +2234,1700 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E6F1F5-4CE9-414F-86C2-1BFBDD82ACCF}">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128:XFD141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="43.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="103.83203125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="43.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D1" t="s">
-        <v>366</v>
-      </c>
-      <c r="E1" t="s">
-        <v>367</v>
+        <v>298</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>325</v>
+        <v>579</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>325</v>
+        <v>579</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>323</v>
+        <v>317</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>337</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D20" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="187" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>338</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>147</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="D36" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>148</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="D37" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>149</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>150</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>331</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>345</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="D38" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>151</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="D39" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="D40" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>153</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="B41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="D41" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>154</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="D42" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>155</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B43" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="D43" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>156</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="D44" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>157</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="D45" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>158</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="D46" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>159</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="B47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="D47" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>160</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B48" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="D48" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>161</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="D49" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>162</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B50" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="D50" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>163</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="B51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="D51" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>164</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="B52" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="D52" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>165</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="B53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="D53" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>166</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="B54" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="D54" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>167</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="B55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="D55" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="D56" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>169</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="B57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="D57" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>170</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="D58" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>171</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="B59" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>172</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>172</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="D60" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>173</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="D61" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>175</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>174</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="D63" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>176</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>175</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="D64" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>177</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>176</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>177</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>178</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>179</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>180</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>181</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D65" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>1</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>2</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>3</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>4</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>5</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>6</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>7</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>8</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>9</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>10</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>11</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>12</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>13</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>14</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>15</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>16</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>17</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>18</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>19</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>20</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="153" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>21</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>22</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>23</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>24</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>25</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>306</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>26</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>27</v>
       </c>
@@ -2638,304 +3935,472 @@
         <v>49</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>28</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>29</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>30</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>31</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>32</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>33</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>34</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>35</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>36</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>37</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>38</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>39</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>40</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>41</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>42</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>333</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>341</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>180</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>181</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C119" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>182</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>353</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>183</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>184</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>185</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>186</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>340</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>348</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>184</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C118" s="1" t="s">
+      <c r="D125" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>187</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>185</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>186</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>360</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>187</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="D126" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>188</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>189</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>190</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>191</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>192</v>
-      </c>
       <c r="B127" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>